<commit_message>
Need to fix: Authorize to get/update/delete coupons
</commit_message>
<xml_diff>
--- a/coupons.xlsx
+++ b/coupons.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Code</t>
   </si>
@@ -38,19 +38,31 @@
     <t>LimitedUseNum</t>
   </si>
   <si>
+    <t>aaaaaaaAAAA</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>13/11/2024</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>BOAZ123</t>
   </si>
   <si>
     <t>ttt</t>
   </si>
   <si>
-    <t>11/11/2024</t>
-  </si>
-  <si>
     <t>21/11/2024</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>coupon</t>
   </si>
 </sst>
 </file>
@@ -97,13 +109,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.928135871887207" customWidth="1"/>
     <col min="2" max="2" width="10.727521896362305" customWidth="1"/>
     <col min="3" max="3" width="16.70222282409668" customWidth="1"/>
     <col min="4" max="4" width="11.43445873260498" customWidth="1"/>
@@ -150,19 +162,71 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="0">
         <v>20</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="0">
-        <v>20</v>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>